<commit_message>
vi hoisting, boolean, true and false
</commit_message>
<xml_diff>
--- a/javascript anotaciones.xlsx
+++ b/javascript anotaciones.xlsx
@@ -9,10 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="scope" sheetId="2" r:id="rId2"/>
+    <sheet name="hoisting" sheetId="3" r:id="rId3"/>
+    <sheet name="coercion" sheetId="4" r:id="rId4"/>
+    <sheet name="truthy and falsy" sheetId="5" r:id="rId5"/>
+    <sheet name="operadores asigancion comp arit" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,12 +28,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>curso recomendado</t>
+  </si>
+  <si>
+    <t>coercion implicita</t>
+  </si>
+  <si>
+    <t>coercion explicita</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,6 +349,254 @@
         <a:xfrm>
           <a:off x="9906000" y="3238500"/>
           <a:ext cx="2066925" cy="2543175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238584</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3286584" cy="3086531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>124480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="190500"/>
+          <a:ext cx="4696480" cy="2295845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>334272</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38371</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6430272" cy="1943371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390899</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95689</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2676899" cy="3143689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>715219</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>105508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3619500"/>
+          <a:ext cx="6049219" cy="5249008"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190945</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>105428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="0"/>
+          <a:ext cx="3191320" cy="4677428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -597,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -606,4 +882,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:I22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vi clases; arrays, condicionales if else, switch
</commit_message>
<xml_diff>
--- a/javascript anotaciones.xlsx
+++ b/javascript anotaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="coercion" sheetId="4" r:id="rId4"/>
     <sheet name="truthy and falsy" sheetId="5" r:id="rId5"/>
     <sheet name="operadores asigancion comp arit" sheetId="6" r:id="rId6"/>
+    <sheet name="condicion if else" sheetId="7" r:id="rId7"/>
+    <sheet name="switch" sheetId="8" r:id="rId8"/>
+    <sheet name="array" sheetId="9" r:id="rId9"/>
+    <sheet name="loops for y for of" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>curso recomendado</t>
   </si>
@@ -39,12 +43,30 @@
   <si>
     <t>coercion explicita</t>
   </si>
+  <si>
+    <t>reto pero esta mal el codigo</t>
+  </si>
+  <si>
+    <t>aquí saque una fruta</t>
+  </si>
+  <si>
+    <t>aquí se agrega un elemento al principio de la lista</t>
+  </si>
+  <si>
+    <t>aquí agregue una frutaal final de la lista</t>
+  </si>
+  <si>
+    <t>asi se quita elementos en arrays "al principio de la lista"</t>
+  </si>
+  <si>
+    <t>/* asi se busca la posicion de los elemntos*/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +82,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,9 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,6 +642,634 @@
         <a:xfrm>
           <a:off x="47625" y="0"/>
           <a:ext cx="3191320" cy="4677428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>638583</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>86561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="2924583" cy="5992061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>162373</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="190500"/>
+          <a:ext cx="3210373" cy="2514951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219599</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>67199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="2790825"/>
+          <a:ext cx="3753374" cy="3753374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>724426</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3772426" cy="2991267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571860</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66989</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4086225" y="104775"/>
+          <a:ext cx="2581635" cy="2248214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581638</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19744</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="190500"/>
+          <a:ext cx="4391638" cy="4972744"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>410164</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>114741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6477000"/>
+          <a:ext cx="4220164" cy="3162741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381585</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>134007</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4191585" cy="4706007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>429110</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>105508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="0"/>
+          <a:ext cx="3477110" cy="5249008"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>105428</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>124401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4677428" cy="4124901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>588</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6457950" y="647700"/>
+          <a:ext cx="4210638" cy="2934109"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>667322</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="4162425"/>
+          <a:ext cx="4096322" cy="2448267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>305374</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="6858000"/>
+          <a:ext cx="4115374" cy="3410426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="4848225"/>
+          <a:ext cx="3762900" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>29004</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6629400"/>
+          <a:ext cx="3077004" cy="876422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476742</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>47796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6629400"/>
+          <a:ext cx="3524742" cy="1228896"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -884,6 +1557,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -903,7 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -964,12 +1649,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A8:O39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vi swith, loops ciclos, objetos, while
</commit_message>
<xml_diff>
--- a/javascript anotaciones.xlsx
+++ b/javascript anotaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,11 @@
     <sheet name="condicion if else" sheetId="7" r:id="rId7"/>
     <sheet name="switch" sheetId="8" r:id="rId8"/>
     <sheet name="array" sheetId="9" r:id="rId9"/>
-    <sheet name="loops for y for of" sheetId="10" r:id="rId10"/>
+    <sheet name="loops for y for of ciclo" sheetId="10" r:id="rId10"/>
+    <sheet name="while" sheetId="11" r:id="rId11"/>
+    <sheet name="objetos" sheetId="12" r:id="rId12"/>
+    <sheet name="objts fncion constructora" sheetId="13" r:id="rId13"/>
+    <sheet name="metodo reorrido array" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>curso recomendado</t>
   </si>
@@ -60,6 +64,21 @@
   </si>
   <si>
     <t>/* asi se busca la posicion de los elemntos*/</t>
+  </si>
+  <si>
+    <t>ciclos</t>
+  </si>
+  <si>
+    <t>primera manera</t>
+  </si>
+  <si>
+    <t>segunda manera</t>
+  </si>
+  <si>
+    <t>viendolo paso a apso</t>
+  </si>
+  <si>
+    <t>propiedad; metodos de objetos</t>
   </si>
 </sst>
 </file>
@@ -122,11 +141,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,6 +416,444 @@
         <a:xfrm>
           <a:off x="9906000" y="3238500"/>
           <a:ext cx="2066925" cy="2543175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>191377</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="6287377" cy="3029373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>515273</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114635</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="571500"/>
+          <a:ext cx="6611273" cy="2400635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>458117</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6838950" y="3971925"/>
+          <a:ext cx="6573167" cy="2391109"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>601010</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6697010" cy="3029373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>58107</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>143382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677150" y="2038350"/>
+          <a:ext cx="6858957" cy="3629532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>695897</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>162586</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8029575" y="0"/>
+          <a:ext cx="4096322" cy="4734586"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371952</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3419952" cy="3162741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>715038</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="4114800"/>
+          <a:ext cx="4753638" cy="2419688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>153039</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>86136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142875" y="381000"/>
+          <a:ext cx="4582164" cy="2943636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>505399</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="3419475"/>
+          <a:ext cx="4115374" cy="543001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>524440</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285750" y="3962400"/>
+          <a:ext cx="4048690" cy="543001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1559,6 +2019,95 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="10" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
culmine el curso javascriptbaico recorridos de aray, proximo curso a verr; fundamentos javascript, v8 y el navegador, ecmascript 6
</commit_message>
<xml_diff>
--- a/javascript anotaciones.xlsx
+++ b/javascript anotaciones.xlsx
@@ -25,7 +25,7 @@
     <sheet name="while" sheetId="11" r:id="rId11"/>
     <sheet name="objetos" sheetId="12" r:id="rId12"/>
     <sheet name="objts fncion constructora" sheetId="13" r:id="rId13"/>
-    <sheet name="metodo reorrido array" sheetId="14" r:id="rId14"/>
+    <sheet name="metodo recorrido array" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>curso recomendado</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>propiedad; metodos de objetos</t>
+  </si>
+  <si>
+    <t>https://jsconsole.com/</t>
+  </si>
+  <si>
+    <t>.map</t>
+  </si>
+  <si>
+    <t>.filtro</t>
+  </si>
+  <si>
+    <t>.find</t>
+  </si>
+  <si>
+    <t>.forEach</t>
+  </si>
+  <si>
+    <t>.some</t>
+  </si>
+  <si>
+    <t>este solo regresa un true o flase es solo para validar una informacion</t>
   </si>
 </sst>
 </file>
@@ -173,53 +194,53 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>48147</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57392</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="609600"/>
+          <a:ext cx="3743847" cy="1733792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>333897</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114542</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="400050" y="285750"/>
-          <a:ext cx="3743847" cy="1733792"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -234,7 +255,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4486275" y="209550"/>
+          <a:off x="4362450" y="304800"/>
           <a:ext cx="3200400" cy="2914650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -247,15 +268,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -270,7 +291,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7886700" y="123825"/>
+          <a:off x="7981950" y="571500"/>
           <a:ext cx="3419475" cy="2333625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -854,6 +875,420 @@
         <a:xfrm>
           <a:off x="285750" y="3962400"/>
           <a:ext cx="4048690" cy="543001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>134386</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>67486</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect t="8524"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="85725"/>
+          <a:ext cx="7421011" cy="5315761"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="2524125"/>
+          <a:ext cx="7134225" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>448588</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>29403</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6286500"/>
+          <a:ext cx="6544588" cy="5934903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Elipse 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9858375"/>
+          <a:ext cx="7134225" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Elipse 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11363325"/>
+          <a:ext cx="7134225" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>610317</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>57657</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="12620625"/>
+          <a:ext cx="5134692" cy="3629532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Elipse 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12592050"/>
+          <a:ext cx="7134225" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>162586</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>67243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16764000"/>
+          <a:ext cx="4734586" cy="4067743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>124480</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>124161</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21336000"/>
+          <a:ext cx="4696480" cy="2410161"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2004,14 +2439,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2108,13 +2549,48 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="H14:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H122" sqref="H122"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="14" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I71" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H116" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H118" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2250,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>